<commit_message>
actualiza notas estudiantes taller2
</commit_message>
<xml_diff>
--- a/MONITOR/2021-2/Taller2/Estudiantes.xlsx
+++ b/MONITOR/2021-2/Taller2/Estudiantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UJ\UJ2021-01\Monitorias\revisionTrabajos\MONITOR\2021-2\Taller2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E769213-9E28-47D6-B2F0-041FA0EF8939}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94CA0F5-AA74-4472-B76A-9B312C1E484D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,6 +421,12 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -441,12 +447,6 @@
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4373,7 +4373,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E10" sqref="E10"/>
+      <selection pane="topRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -4386,22 +4386,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" customHeight="1" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:14" ht="18" customHeight="1" thickBot="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="20" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="22" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4421,32 +4421,32 @@
       <c r="E3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="18" t="s">
+      <c r="F3" s="22"/>
+      <c r="G3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
     </row>
     <row r="4" spans="1:14" ht="16.5" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="15">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="15">
         <v>10</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="15">
         <v>10</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="15">
         <v>9.8000000000000007</v>
       </c>
       <c r="F4" s="10"/>
@@ -4487,10 +4487,18 @@
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="B7" s="6">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6">
+        <v>10</v>
+      </c>
+      <c r="E7" s="6">
+        <v>10</v>
+      </c>
       <c r="F7" s="10"/>
       <c r="G7" s="8"/>
       <c r="H7" s="12"/>
@@ -4515,10 +4523,18 @@
       <c r="A9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="B9" s="6">
+        <v>7.8</v>
+      </c>
+      <c r="C9" s="6">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D9" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="E9" s="6">
+        <v>6.8</v>
+      </c>
       <c r="F9" s="10"/>
       <c r="G9" s="8"/>
       <c r="H9" s="12"/>
@@ -4593,16 +4609,16 @@
       <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="15">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="15">
         <v>10</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="15">
         <v>10</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="15">
         <v>10</v>
       </c>
       <c r="F14" s="10"/>
@@ -4615,10 +4631,18 @@
       <c r="A15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="B15" s="6">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C15" s="6">
+        <v>9.6</v>
+      </c>
+      <c r="D15" s="6">
+        <v>9.6</v>
+      </c>
+      <c r="E15" s="6">
+        <v>8.6</v>
+      </c>
       <c r="F15" s="10"/>
       <c r="G15" s="8"/>
       <c r="H15" s="12"/>
@@ -4673,10 +4697,18 @@
       <c r="A18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="B18" s="6">
+        <v>9.4</v>
+      </c>
+      <c r="C18" s="6">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D18" s="6">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E18" s="6">
+        <v>10</v>
+      </c>
       <c r="F18" s="10"/>
       <c r="G18" s="8"/>
       <c r="H18" s="12"/>
@@ -4709,10 +4741,18 @@
       <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="B20" s="6">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C20" s="6">
+        <v>10</v>
+      </c>
+      <c r="D20" s="6">
+        <v>10</v>
+      </c>
+      <c r="E20" s="6">
+        <v>10</v>
+      </c>
       <c r="F20" s="10"/>
       <c r="G20" s="8"/>
       <c r="H20" s="12"/>
@@ -4723,7 +4763,7 @@
       <c r="A21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="16">
         <v>10</v>
       </c>
       <c r="C21" s="6">

</xml_diff>